<commit_message>
feat: Sistema completo plantillas Excel y carga masiva empleados - TFG Final
</commit_message>
<xml_diff>
--- a/empleados_ejemplo.xlsx
+++ b/empleados_ejemplo.xlsx
@@ -427,19 +427,19 @@
         <v>Ana García Rodríguez</v>
       </c>
       <c r="B2" t="str">
-        <v>ana.garcia@empresa.com</v>
+        <v>ana.garcia@hackless.com</v>
       </c>
       <c r="C2" t="str">
         <v>empleado</v>
       </c>
       <c r="D2" t="str">
-        <v>Operador de Planta</v>
+        <v>Operadora de Línea de Producción</v>
       </c>
       <c r="E2" t="str">
         <v>Producción</v>
       </c>
       <c r="F2" t="str">
-        <v>011-4567-8901</v>
+        <v>+54 9 11 1234-5678</v>
       </c>
     </row>
     <row r="3">
@@ -447,79 +447,79 @@
         <v>Carlos López Martínez</v>
       </c>
       <c r="B3" t="str">
-        <v>carlos.lopez@empresa.com</v>
+        <v>carlos.lopez@hackless.com</v>
       </c>
       <c r="C3" t="str">
         <v>supervisor</v>
       </c>
       <c r="D3" t="str">
-        <v>Supervisor de Seguridad</v>
+        <v>Supervisor de Seguridad Industrial</v>
       </c>
       <c r="E3" t="str">
         <v>Seguridad e Higiene</v>
       </c>
       <c r="F3" t="str">
-        <v>011-4567-8902</v>
+        <v>+54 9 11 2345-6789</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>María Fernández Silva</v>
+        <v>María José Fernández</v>
       </c>
       <c r="B4" t="str">
-        <v>maria.fernandez@empresa.com</v>
+        <v>maria.fernandez@hackless.com</v>
       </c>
       <c r="C4" t="str">
         <v>administrador</v>
       </c>
       <c r="D4" t="str">
-        <v>Jefe de RRHH</v>
+        <v>Jefe de Recursos Humanos</v>
       </c>
       <c r="E4" t="str">
-        <v>Recursos Humanos</v>
+        <v>Administración</v>
       </c>
       <c r="F4" t="str">
-        <v>011-4567-8903</v>
+        <v>+54 9 11 3456-7890</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Juan Pedro Sánchez</v>
+        <v>Juan Carlos Sánchez</v>
       </c>
       <c r="B5" t="str">
-        <v>juan.sanchez@empresa.com</v>
+        <v>juan.sanchez@hackless.com</v>
       </c>
       <c r="C5" t="str">
         <v>empleado</v>
       </c>
       <c r="D5" t="str">
-        <v>Técnico de Mantenimiento</v>
+        <v>Técnico en Mantenimiento Mecánico</v>
       </c>
       <c r="E5" t="str">
         <v>Mantenimiento</v>
       </c>
       <c r="F5" t="str">
-        <v>011-4567-8904</v>
+        <v>+54 9 11 4567-8901</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Laura Morales Vega</v>
+        <v>Laura Patricia Morales</v>
       </c>
       <c r="B6" t="str">
-        <v>laura.morales@empresa.com</v>
+        <v>laura.morales@hackless.com</v>
       </c>
       <c r="C6" t="str">
         <v>auditor</v>
       </c>
       <c r="D6" t="str">
-        <v>Auditor Interno</v>
+        <v>Auditor Interno de Calidad</v>
       </c>
       <c r="E6" t="str">
         <v>Calidad</v>
       </c>
       <c r="F6" t="str">
-        <v>011-4567-8905</v>
+        <v>+54 9 11 5678-9012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>